<commit_message>
tfs10524 - ecl move db file shares
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C39798
</commit_message>
<xml_diff>
--- a/Requirements/Misc/CCO_eCL_Test_Job_Steps.xlsx
+++ b/Requirements/Misc/CCO_eCL_Test_Job_Steps.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a_wip\ecl\doc\tfs_changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Requirements\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>Step Name</t>
   </si>
@@ -74,12 +74,6 @@
   </si>
   <si>
     <t>WHFileLoad</t>
-  </si>
-  <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching\Outliers\Test\eCl_Outlier_Feed_&lt;ReportCode&gt;&lt;CCYYMMDD&gt;.csv</t>
-  </si>
-  <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching\ETS\Test\eCL_ETS_Feed_&lt;ReportCode&gt;&lt;CCYYMMDD&gt;.csv</t>
   </si>
   <si>
     <t>EC.Coaching_Log.EmailSent = 0 or null</t>
@@ -97,12 +91,6 @@
     <t>Inactivations</t>
   </si>
   <si>
-    <t>EC.Coaching_Log.StatusID = 2 or
-EC.Warning_Log.StatusID = 2
-email notification sent to john;
-log file generated to \\vrivscors01\BCC Scorecards\Coaching\Inactivations\Processed</t>
-  </si>
-  <si>
     <t>CoachingReminders</t>
   </si>
   <si>
@@ -174,11 +162,6 @@
   </si>
   <si>
     <t>EC.Survey_Response_Header.NotificationDate = today's date - 3</t>
-  </si>
-  <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching\EmpInfo\Test\Employee_Information_WithProgram.csv
-\\vrivscors01\BCC Scorecards\Coaching\HRInfo\Test\PS_Employee_Information_&lt;MMDDCCYY&gt;.csv
-\\vrivscors01\BCC Scorecards\Coaching\HRInfo\Test\HR_Employee_Information.csv</t>
   </si>
   <si>
     <t>EC.ETS_Coaching_Filelist
@@ -189,9 +172,6 @@
         EC.Coaching_Log_Reason</t>
   </si>
   <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching\Generic\Test\eCL_Generic_Feed_XXX[_ZZZ]&lt;YYYYMMDD&gt;.csv</t>
-  </si>
-  <si>
     <t>EC.Generic_Coaching_Filelist
 EC.Generic_Coaching_Stage
     EC.Generic_Coaching_Rejected
@@ -208,9 +188,6 @@
         EC.Coaching_Log_Reason</t>
   </si>
   <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching\Apps\Encryption\Encrypt_out\Test_eCL_IQS_Scorecard_&lt;CCYYMMDD&gt;.csv.zip.encrypt</t>
-  </si>
-  <si>
     <t>EC.Quality_Coaching_Filelist
 EC.Quality_Coaching_Stage
     EC.Quality_Coacing_Rejected
@@ -219,9 +196,6 @@
         EC.Coaching_Log_Reason</t>
   </si>
   <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching\Quality\Test\eCL_Quality_Feed_XXX&lt;YYYYMMDD&gt;.csv</t>
-  </si>
-  <si>
     <t>EC.Quality_Other_Coaching_Filelist
 EC.Quality_Other_Coaching_Stage
     EC.Quality_Other_Coacing_Rejected
@@ -230,9 +204,6 @@
         EC.Coaching_Log_Reason</t>
   </si>
   <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching\Training\Test\eCL_Training_Feed_XXX&lt;YYYYMMDD&gt;.csv</t>
-  </si>
-  <si>
     <t>EC.Training_Coaching_Filelist
 EC.Training_Coaching_Stage
     EC.Training_Coacing_Rejected
@@ -247,9 +218,6 @@
     <t>Input Data Feed</t>
   </si>
   <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching\WH\Test\&lt;SiteLocation&gt;Warnings.csv</t>
-  </si>
-  <si>
     <t>EC.Warning_History_Filelist
 EC.Warning_History_Stage
     EC.Warning_History_Rejected
@@ -282,10 +250,6 @@
 EC.Survey_Response_Detail</t>
   </si>
   <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching\Inactivations\Test\eCL_Coaching_&lt;MMDDCCYY&gt;.csv
-\\vrivscors01\BCC Scorecards\Coaching\Inactivations\Test\eCL_Warning_&lt;MMDDCCYY&gt;.csv</t>
-  </si>
-  <si>
     <t>One time history load - No longer used</t>
   </si>
   <si>
@@ -326,6 +290,38 @@
   <si>
     <t>Inactivations logs
 source - supervisor/manager in operations</t>
+  </si>
+  <si>
+    <t>\\F3420-ECLDBP01\data\Coaching\Outliers\Encrypt_In\eCl_Outlier_Feed_&lt;ReportCode&gt;&lt;CCYYMMDD&gt;.csv.zip.encrypt</t>
+  </si>
+  <si>
+    <t>\\F3420-ECLDBP01\data\Coaching\IQS\Encrypt_In\eCL_IQS_Scorecard_&lt;CCYYMMDD&gt;.csv.zip.encrypt</t>
+  </si>
+  <si>
+    <t>\\F3420-ECLDBP01\data\Coaching\ETS\Encrypt_In\eCL_ETS_Feed_&lt;ReportCode&gt;&lt;CCYYMMDD&gt;.csv.zip.encrypt</t>
+  </si>
+  <si>
+    <t>\\F3420-ECLDBP01\data\Coaching\Training\Encrypt_In\eCL_Training_Feed_XXX&lt;YYYYMMDD&gt;.csv.zip.encrypt</t>
+  </si>
+  <si>
+    <t>\\F3420-ECLDBP01\data\Coaching\Generic\Encrypt_In\eCL_Generic_Feed_XXX[_ZZZ]&lt;YYYYMMDD&gt;.csv.zip.encrypt</t>
+  </si>
+  <si>
+    <t>\\F3420-ECLDBP01\data\Coaching\Quality\Encrypt_In\eCL_Quality_Feed_XXX&lt;YYYYMMDD&gt;.csv.zip.encrypt</t>
+  </si>
+  <si>
+    <t>\\F3420-ECLDBP01\Data\Coaching\HRInfo\Encrypt_In\Employee_Information_WithProgram.csv.zip.encrypt
+\\vrivscors01\BCC \\F3420-ECLDBP01\Data\Coaching\HRInfo\Encrypt_In\PS_Employee_Information_&lt;MMDDCCYY&gt;.csv.zip.encrypt
+\\F3420-ECLDBP01\Data\Coaching\HRInfo\Encrypt_In\HR_Employee_Information.csv.zip.encrypt</t>
+  </si>
+  <si>
+    <t>legacy - no longer used</t>
+  </si>
+  <si>
+    <t>EC.Coaching_Log.StatusID = 2 or
+EC.Warning_Log.StatusID = 2
+email notification sent to john;
+log file generated to &lt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -750,7 +746,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>4</v>
@@ -770,7 +766,7 @@
     </row>
     <row r="2" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -779,13 +775,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -798,7 +794,7 @@
     </row>
     <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -807,13 +803,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -826,22 +822,22 @@
     </row>
     <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -854,7 +850,7 @@
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>9</v>
@@ -863,13 +859,13 @@
         <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -882,7 +878,7 @@
     </row>
     <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>10</v>
@@ -891,13 +887,13 @@
         <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -910,22 +906,22 @@
     </row>
     <row r="12" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -938,22 +934,22 @@
     </row>
     <row r="14" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -966,7 +962,7 @@
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>8</v>
@@ -978,10 +974,10 @@
         <v>14</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -994,22 +990,22 @@
     </row>
     <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1022,22 +1018,22 @@
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1050,22 +1046,22 @@
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="E22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1078,22 +1074,22 @@
     </row>
     <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1106,7 +1102,7 @@
     </row>
     <row r="26" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>11</v>
@@ -1115,13 +1111,13 @@
         <v>17</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1132,24 +1128,24 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
tfs15984 - ecl update overview documents
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C44008
</commit_message>
<xml_diff>
--- a/Requirements/Misc/CCO_eCL_Test_Job_Steps.xlsx
+++ b/Requirements/Misc/CCO_eCL_Test_Job_Steps.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Requirements\Misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS_Omni\eCoaching_V2\Requirements\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
   <si>
     <t>Step Name</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Individual Job Name</t>
   </si>
   <si>
-    <t>CoachingEmployeeLoadNew</t>
-  </si>
-  <si>
     <t>EmployeeLoad</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>CoachingQualityLoad</t>
   </si>
   <si>
-    <t>CoachingWHLoad</t>
-  </si>
-  <si>
     <t>ETSFileLoad</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
   </si>
   <si>
     <t>IQSLoad</t>
-  </si>
-  <si>
-    <t>WHFileLoad</t>
   </si>
   <si>
     <t>EC.Coaching_Log.EmailSent = 0 or null</t>
@@ -83,12 +74,6 @@
     EC.Employee_Hierarchy
     EC.EmployeeID_To_LanID
     EC.CSR_Hierarchy</t>
-  </si>
-  <si>
-    <t>CoachingInactivations</t>
-  </si>
-  <si>
-    <t>Inactivations</t>
   </si>
   <si>
     <t>CoachingReminders</t>
@@ -218,14 +203,6 @@
     <t>Input Data Feed</t>
   </si>
   <si>
-    <t>EC.Warning_History_Filelist
-EC.Warning_History_Stage
-    EC.Warning_History_Rejected
-    EC.Warning_History_Fact
-        EC.Warning_Log
-        EC.Warning_Log_Reason</t>
-  </si>
-  <si>
     <t>Sends emails</t>
   </si>
   <si>
@@ -250,12 +227,6 @@
 EC.Survey_Response_Detail</t>
   </si>
   <si>
-    <t>One time history load - No longer used</t>
-  </si>
-  <si>
-    <t>Process - No longer used</t>
-  </si>
-  <si>
     <t>Imports user information into staging tables
 source - aspect/wfm, people soft/hr, hr/hr</t>
   </si>
@@ -282,14 +253,6 @@
   <si>
     <t>Imports training reports information to create coaching logs
 source - training reports</t>
-  </si>
-  <si>
-    <t>Imports information to create warning logs
-source - hr and operations</t>
-  </si>
-  <si>
-    <t>Inactivations logs
-source - supervisor/manager in operations</t>
   </si>
   <si>
     <t>\\F3420-ECLDBP01\data\Coaching\Outliers\Encrypt_In\eCl_Outlier_Feed_&lt;ReportCode&gt;&lt;CCYYMMDD&gt;.csv.zip.encrypt</t>
@@ -315,13 +278,64 @@
 \\F3420-ECLDBP01\Data\Coaching\HRInfo\Encrypt_In\HR_Employee_Information.csv.zip.encrypt</t>
   </si>
   <si>
-    <t>legacy - no longer used</t>
-  </si>
-  <si>
-    <t>EC.Coaching_Log.StatusID = 2 or
-EC.Warning_Log.StatusID = 2
-email notification sent to john;
-log file generated to &lt;&gt;</t>
+    <t>CoachingEmployeeHierarchyLoad</t>
+  </si>
+  <si>
+    <t>CoachingFollowUpNotifications</t>
+  </si>
+  <si>
+    <t>Sends emails to coaching log reviewers when follow-up date is reached</t>
+  </si>
+  <si>
+    <t>selection determined by whether follow-up is required, status is pending follow-up, follow-up date is reached</t>
+  </si>
+  <si>
+    <t>EC.Coaching_Log.IsFollowupRequired=1,
+EC.Coaching_Log.FollowupDueDate = current date,
+email notification sent to supervisor</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>CoachingIISLogImport</t>
+  </si>
+  <si>
+    <t>eCoaching Log Usage reporting</t>
+  </si>
+  <si>
+    <t>Imports IIS logs for reporting</t>
+  </si>
+  <si>
+    <t>CoachingQualityNowLoad</t>
+  </si>
+  <si>
+    <t>Imports IQS Quality Now information to create coaching logs
+source - iqs/quality</t>
+  </si>
+  <si>
+    <t>EC.Quality_Now_Coaching_Filelist
+EC.Quality_Now_Coaching_Stage
+    EC.Quality_Now_Coacing_Rejected
+    EC.Quality_Now_Coaching_Fact
+        EC.Coaching_Log
+        EC.Coaching_Log_Reason
+        EC.Coaching_Quality_Now_Evaluations</t>
+  </si>
+  <si>
+    <t>CoachingSummaryReport</t>
+  </si>
+  <si>
+    <t>Coaching Log Summary Report</t>
+  </si>
+  <si>
+    <t>Creates a report of coaching logs</t>
+  </si>
+  <si>
+    <t>Coaching log tables</t>
+  </si>
+  <si>
+    <t>\\F3420-ECLDBT01\Data\Coaching\Reports</t>
   </si>
 </sst>
 </file>
@@ -345,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,12 +375,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -421,10 +429,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -731,13 +735,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" customWidth="1"/>
     <col min="5" max="5" width="55.6640625" customWidth="1"/>
@@ -746,7 +752,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>4</v>
@@ -766,22 +772,22 @@
     </row>
     <row r="2" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -794,22 +800,22 @@
     </row>
     <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -820,24 +826,24 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -850,22 +856,22 @@
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -876,49 +882,45 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>76</v>
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>49</v>
@@ -934,22 +936,22 @@
     </row>
     <row r="14" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -960,52 +962,52 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1016,24 +1018,24 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1044,24 +1046,24 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1072,24 +1074,24 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1100,23 +1102,23 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="11" t="s">
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1124,37 +1126,93 @@
       <c r="A27" s="8"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>79</v>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>